<commit_message>
Enhance structure of mapping, added SQLLite database to store ohlcv data
</commit_message>
<xml_diff>
--- a/src/main/resources/IBM_daily.xlsx
+++ b/src/main/resources/IBM_daily.xlsx
@@ -22,6 +22,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="2548">
   <si>
+    <t xml:space="preserve">IBM daily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
@@ -38,12 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IBM daily</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> yyyy/MM/dd</t>
   </si>
   <si>
     <t xml:space="preserve">2018/01/05</t>
@@ -7678,6 +7678,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7762,14 +7763,14 @@
   <dimension ref="A1:F508"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -7778,27 +7779,30 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>